<commit_message>
feat: implemented card counting
</commit_message>
<xml_diff>
--- a/src/main/resources/strategies/CustomCardCounting.xlsx
+++ b/src/main/resources/strategies/CustomCardCounting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\BlackjackSimulator\src\main\resources\strategies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3C7FA9-A310-4500-BC7B-C8C7651EC5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A22F8B6-F22B-4421-8F67-2BE262B828E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{21CDB781-D789-4925-8E21-207DEAF49322}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="23">
   <si>
     <t>Outcome</t>
   </si>
@@ -19283,7 +19283,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19292,8 +19292,8 @@
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
+      <c r="B1">
+        <v>11</v>
       </c>
       <c r="C1">
         <v>2</v>
@@ -19466,7 +19466,7 @@
   <dimension ref="A1:BH19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19523,31 +19523,31 @@
         <v>0.35360813639536137</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:I3" si="0">C13</f>
+        <f t="shared" ref="C3" si="0">C13</f>
         <v>0.3738748853821432</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
+        <f>D13</f>
         <v>0.39446844550254284</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f>E13</f>
         <v>0.41640366958226238</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
+        <f>F13</f>
         <v>0.42315049208499783</v>
       </c>
       <c r="G3">
-        <f t="shared" si="0"/>
+        <f>G13</f>
         <v>0.26231240836153336</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
+        <f>H13</f>
         <v>0.2447412422511914</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
+        <f>I13</f>
         <v>0.2284251594344453</v>
       </c>
       <c r="J3">
@@ -19564,35 +19564,35 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:I4" si="1">B14</f>
+        <f>B14</f>
         <v>0.13980913952773527</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
+        <f>C14</f>
         <v>0.13503398781113993</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
+        <f>D14</f>
         <v>0.13048973584959825</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
+        <f>E14</f>
         <v>0.12225128527055079</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
+        <f>F14</f>
         <v>0.16543817650334638</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f>G14</f>
         <v>0.36856619379423861</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f>H14</f>
         <v>0.12856654444917001</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f>I14</f>
         <v>0.119995441485892</v>
       </c>
       <c r="J4">
@@ -19609,35 +19609,35 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:I5" si="2">B15</f>
+        <f>B15</f>
         <v>0.13490735037469442</v>
       </c>
       <c r="C5">
-        <f t="shared" si="2"/>
+        <f>C15</f>
         <v>0.13048232645474483</v>
       </c>
       <c r="D5">
-        <f t="shared" si="2"/>
+        <f>D15</f>
         <v>0.12593807449320316</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
+        <f>E15</f>
         <v>0.12225128527055079</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
+        <f>F15</f>
         <v>0.10626657887021028</v>
       </c>
       <c r="G5">
-        <f t="shared" si="2"/>
+        <f>G15</f>
         <v>0.13779696302500785</v>
       </c>
       <c r="H5">
-        <f t="shared" si="2"/>
+        <f>H15</f>
         <v>0.35933577521840082</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f>I15</f>
         <v>0.119995441485892</v>
       </c>
       <c r="J5">
@@ -19654,35 +19654,35 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:I6" si="3">B16</f>
+        <f>B16</f>
         <v>0.12965543342500779</v>
       </c>
       <c r="C6">
-        <f t="shared" si="3"/>
+        <f>C16</f>
         <v>0.12558053730170399</v>
       </c>
       <c r="D6">
-        <f t="shared" si="3"/>
+        <f>D16</f>
         <v>0.12138641313680808</v>
       </c>
       <c r="E6">
-        <f t="shared" si="3"/>
+        <f>E16</f>
         <v>0.11769962391415568</v>
       </c>
       <c r="F6">
-        <f t="shared" si="3"/>
+        <f>F16</f>
         <v>0.10626657887021028</v>
       </c>
       <c r="G6">
-        <f t="shared" si="3"/>
+        <f>G16</f>
         <v>7.8625365391871746E-2</v>
       </c>
       <c r="H6">
-        <f t="shared" si="3"/>
+        <f>H16</f>
         <v>0.12856654444917001</v>
       </c>
       <c r="I6">
-        <f t="shared" si="3"/>
+        <f>I16</f>
         <v>0.35076467225512281</v>
       </c>
       <c r="J6">
@@ -19699,35 +19699,35 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7:I7" si="4">B17</f>
+        <f>B17</f>
         <v>0.12402645577124111</v>
       </c>
       <c r="C7">
-        <f t="shared" si="4"/>
+        <f>C17</f>
         <v>0.12032862035201736</v>
       </c>
       <c r="D7">
-        <f t="shared" si="4"/>
+        <f>D17</f>
         <v>0.1164846239837672</v>
       </c>
       <c r="E7">
-        <f t="shared" si="4"/>
+        <f>E17</f>
         <v>0.11314796255776062</v>
       </c>
       <c r="F7">
-        <f t="shared" si="4"/>
+        <f>F17</f>
         <v>0.1017149175138152</v>
       </c>
       <c r="G7">
-        <f t="shared" si="4"/>
+        <f>G17</f>
         <v>7.8625365391871746E-2</v>
       </c>
       <c r="H7">
-        <f t="shared" si="4"/>
+        <f>H17</f>
         <v>6.9394946816033906E-2</v>
       </c>
       <c r="I7">
-        <f t="shared" si="4"/>
+        <f>I17</f>
         <v>0.119995441485892</v>
       </c>
       <c r="J7">
@@ -19744,35 +19744,35 @@
         <v>21</v>
       </c>
       <c r="B8" s="4">
-        <f t="shared" ref="B8:I8" si="5">B18</f>
+        <f>B18</f>
         <v>0.11799348450596003</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" si="5"/>
+        <f>C18</f>
         <v>0.11469964269825066</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="5"/>
+        <f>D18</f>
         <v>0.11123270703408056</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="5"/>
+        <f>E18</f>
         <v>0.10824617340471974</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" si="5"/>
+        <f>F18</f>
         <v>9.7163256157420108E-2</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" si="5"/>
+        <f>G18</f>
         <v>7.4073704035476667E-2</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="5"/>
+        <f>H18</f>
         <v>6.9394946816033906E-2</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="5"/>
+        <f>I18</f>
         <v>6.0823843852755917E-2</v>
       </c>
       <c r="J8" s="4">
@@ -19793,39 +19793,39 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:K9" si="6">SUM(C3:C8)</f>
+        <f t="shared" ref="C9:K9" si="1">SUM(C3:C8)</f>
         <v>0.99999999999999989</v>
       </c>
       <c r="D9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="E9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="G9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="H9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -19875,178 +19875,178 @@
         <v>11</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" ref="L12:AE12" si="7">K12+1</f>
+        <f t="shared" ref="L12:AE12" si="2">K12+1</f>
         <v>12</v>
       </c>
       <c r="M12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="O12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="P12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="Q12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="R12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="S12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="T12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="U12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="V12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="W12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="X12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="Y12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="Z12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="AA12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="AB12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="AC12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="AD12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="AE12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="AG12" s="4">
         <v>12</v>
       </c>
       <c r="AH12" s="4">
-        <f t="shared" ref="AH12:BH12" si="8">AG12+1</f>
+        <f t="shared" ref="AH12:BH12" si="3">AG12+1</f>
         <v>13</v>
       </c>
       <c r="AI12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="AJ12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="AK12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="AL12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="AM12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="AN12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="AO12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="AP12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="AQ12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="AR12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="AS12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="AT12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="AU12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="AV12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="AW12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="AX12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="AY12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="AZ12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="BE12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="BF12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="BG12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="BH12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
@@ -20169,39 +20169,39 @@
         <v>0.48267271400214928</v>
       </c>
       <c r="AR13">
-        <f t="shared" ref="AR13:AR18" si="9">M13</f>
+        <f t="shared" ref="AR13:AR18" si="4">M13</f>
         <v>0.51962466300199572</v>
       </c>
       <c r="AS13">
-        <f t="shared" ref="AS13:AS18" si="10">N13</f>
+        <f t="shared" ref="AS13:AS18" si="5">N13</f>
         <v>0.55393718707328177</v>
       </c>
       <c r="AT13">
-        <f t="shared" ref="AT13:AT18" si="11">O13</f>
+        <f t="shared" ref="AT13:AT18" si="6">O13</f>
         <v>0.58579881656804733</v>
       </c>
       <c r="AU13">
-        <f t="shared" ref="AU13:AU18" si="12">P13</f>
+        <f t="shared" ref="AU13:AU18" si="7">P13</f>
         <v>0.61538461538461542</v>
       </c>
       <c r="AV13">
-        <f t="shared" ref="AV13:AV18" si="13">Q13</f>
+        <f t="shared" ref="AV13:AV18" si="8">Q13</f>
         <v>0</v>
       </c>
       <c r="AW13">
-        <f t="shared" ref="AW13:AW18" si="14">R13</f>
+        <f t="shared" ref="AW13:AW18" si="9">R13</f>
         <v>0</v>
       </c>
       <c r="AX13">
-        <f t="shared" ref="AX13:AX18" si="15">S13</f>
+        <f t="shared" ref="AX13:AX18" si="10">S13</f>
         <v>0</v>
       </c>
       <c r="AY13">
-        <f t="shared" ref="AY13:AY18" si="16">T13</f>
+        <f t="shared" ref="AY13:AY18" si="11">T13</f>
         <v>0</v>
       </c>
       <c r="AZ13">
-        <f t="shared" ref="AZ13:AZ18" si="17">U13</f>
+        <f>U13</f>
         <v>0</v>
       </c>
     </row>
@@ -20296,43 +20296,43 @@
         <v>1</v>
       </c>
       <c r="AQ14">
-        <f t="shared" ref="AQ14:AQ18" si="18">L14</f>
+        <f t="shared" ref="AQ14:AQ18" si="12">L14</f>
         <v>0.10346545719957015</v>
       </c>
       <c r="AR14">
+        <f t="shared" si="4"/>
+        <v>9.6075067399600853E-2</v>
+      </c>
+      <c r="AS14">
+        <f t="shared" si="5"/>
+        <v>8.9212562585343644E-2</v>
+      </c>
+      <c r="AT14">
+        <f t="shared" si="6"/>
+        <v>8.2840236686390525E-2</v>
+      </c>
+      <c r="AU14">
+        <f t="shared" si="7"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="AV14">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="AW14">
         <f t="shared" si="9"/>
-        <v>9.6075067399600853E-2</v>
-      </c>
-      <c r="AS14">
+        <v>0</v>
+      </c>
+      <c r="AX14">
         <f t="shared" si="10"/>
-        <v>8.9212562585343644E-2</v>
-      </c>
-      <c r="AT14">
+        <v>0</v>
+      </c>
+      <c r="AY14">
         <f t="shared" si="11"/>
-        <v>8.2840236686390525E-2</v>
-      </c>
-      <c r="AU14">
-        <f t="shared" si="12"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-      <c r="AV14">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="AW14">
-        <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AX14">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AY14">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
       <c r="AZ14">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="AZ13:AZ18" si="13">U14</f>
         <v>0</v>
       </c>
     </row>
@@ -20427,43 +20427,43 @@
         <v>1</v>
       </c>
       <c r="AQ15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>0.10346545719957015</v>
       </c>
       <c r="AR15">
+        <f t="shared" si="4"/>
+        <v>9.6075067399600853E-2</v>
+      </c>
+      <c r="AS15">
+        <f t="shared" si="5"/>
+        <v>8.9212562585343644E-2</v>
+      </c>
+      <c r="AT15">
+        <f t="shared" si="6"/>
+        <v>8.2840236686390525E-2</v>
+      </c>
+      <c r="AU15">
+        <f t="shared" si="7"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="AV15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AW15">
         <f t="shared" si="9"/>
-        <v>9.6075067399600853E-2</v>
-      </c>
-      <c r="AS15">
+        <v>1</v>
+      </c>
+      <c r="AX15">
         <f t="shared" si="10"/>
-        <v>8.9212562585343644E-2</v>
-      </c>
-      <c r="AT15">
+        <v>0</v>
+      </c>
+      <c r="AY15">
         <f t="shared" si="11"/>
-        <v>8.2840236686390525E-2</v>
-      </c>
-      <c r="AU15">
-        <f t="shared" si="12"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-      <c r="AV15">
+        <v>0</v>
+      </c>
+      <c r="AZ15">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AW15">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="AX15">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AY15">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AZ15">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -20558,43 +20558,43 @@
         <v>1</v>
       </c>
       <c r="AQ16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>0.10346545719957015</v>
       </c>
       <c r="AR16">
+        <f t="shared" si="4"/>
+        <v>9.6075067399600853E-2</v>
+      </c>
+      <c r="AS16">
+        <f t="shared" si="5"/>
+        <v>8.9212562585343644E-2</v>
+      </c>
+      <c r="AT16">
+        <f t="shared" si="6"/>
+        <v>8.2840236686390525E-2</v>
+      </c>
+      <c r="AU16">
+        <f t="shared" si="7"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="AV16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AW16">
         <f t="shared" si="9"/>
-        <v>9.6075067399600853E-2</v>
-      </c>
-      <c r="AS16">
+        <v>0</v>
+      </c>
+      <c r="AX16">
         <f t="shared" si="10"/>
-        <v>8.9212562585343644E-2</v>
-      </c>
-      <c r="AT16">
+        <v>1</v>
+      </c>
+      <c r="AY16">
         <f t="shared" si="11"/>
-        <v>8.2840236686390525E-2</v>
-      </c>
-      <c r="AU16">
-        <f t="shared" si="12"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-      <c r="AV16">
+        <v>0</v>
+      </c>
+      <c r="AZ16">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AW16">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AX16">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="AY16">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AZ16">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -20689,43 +20689,43 @@
         <v>1</v>
       </c>
       <c r="AQ17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>0.10346545719957015</v>
       </c>
       <c r="AR17">
+        <f t="shared" si="4"/>
+        <v>9.6075067399600853E-2</v>
+      </c>
+      <c r="AS17">
+        <f t="shared" si="5"/>
+        <v>8.9212562585343644E-2</v>
+      </c>
+      <c r="AT17">
+        <f t="shared" si="6"/>
+        <v>8.2840236686390525E-2</v>
+      </c>
+      <c r="AU17">
+        <f t="shared" si="7"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="AV17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AW17">
         <f t="shared" si="9"/>
-        <v>9.6075067399600853E-2</v>
-      </c>
-      <c r="AS17">
+        <v>0</v>
+      </c>
+      <c r="AX17">
         <f t="shared" si="10"/>
-        <v>8.9212562585343644E-2</v>
-      </c>
-      <c r="AT17">
+        <v>0</v>
+      </c>
+      <c r="AY17">
         <f t="shared" si="11"/>
-        <v>8.2840236686390525E-2</v>
-      </c>
-      <c r="AU17">
-        <f t="shared" si="12"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-      <c r="AV17">
+        <v>1</v>
+      </c>
+      <c r="AZ17">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AW17">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AX17">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AY17">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="AZ17">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -20838,43 +20838,43 @@
         <v>1</v>
       </c>
       <c r="AQ18" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>0.10346545719957015</v>
       </c>
       <c r="AR18" s="4">
+        <f t="shared" si="4"/>
+        <v>9.6075067399600853E-2</v>
+      </c>
+      <c r="AS18" s="4">
+        <f t="shared" si="5"/>
+        <v>8.9212562585343644E-2</v>
+      </c>
+      <c r="AT18" s="4">
+        <f t="shared" si="6"/>
+        <v>8.2840236686390525E-2</v>
+      </c>
+      <c r="AU18" s="4">
+        <f t="shared" si="7"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="AV18" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AW18" s="4">
         <f t="shared" si="9"/>
-        <v>9.6075067399600853E-2</v>
-      </c>
-      <c r="AS18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX18" s="4">
         <f t="shared" si="10"/>
-        <v>8.9212562585343644E-2</v>
-      </c>
-      <c r="AT18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY18" s="4">
         <f t="shared" si="11"/>
-        <v>8.2840236686390525E-2</v>
-      </c>
-      <c r="AU18" s="4">
-        <f t="shared" si="12"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-      <c r="AV18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ18" s="4">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AW18" s="4">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AX18" s="4">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AY18" s="4">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AZ18" s="4">
-        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
@@ -20887,199 +20887,199 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:AZ19" si="19">SUM(C13:C18)</f>
+        <f t="shared" ref="C19:AZ19" si="14">SUM(C13:C18)</f>
         <v>0.99999999999999989</v>
       </c>
       <c r="D19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="E19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="F19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="G19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="H19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="I19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="J19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="K19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="L19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="M19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="N19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="O19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="P19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="R19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="S19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="U19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="V19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="W19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="X19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AB19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AC19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AD19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AE19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AG19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="AH19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="AI19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="AJ19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="AK19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AL19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AM19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AN19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AO19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AP19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AQ19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="AR19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="AS19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="AT19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="AU19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="AV19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AW19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AX19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AY19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AZ19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: changed header row from Ace to 11
</commit_message>
<xml_diff>
--- a/src/main/resources/strategies/CustomCardCounting.xlsx
+++ b/src/main/resources/strategies/CustomCardCounting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\BlackjackSimulator\src\main\resources\strategies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A22F8B6-F22B-4421-8F67-2BE262B828E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C4BF01-8F90-4A4D-BF28-32D0FEE8826A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{21CDB781-D789-4925-8E21-207DEAF49322}"/>
+    <workbookView xWindow="0" yWindow="1452" windowWidth="28800" windowHeight="15828" xr2:uid="{21CDB781-D789-4925-8E21-207DEAF49322}"/>
   </bookViews>
   <sheets>
     <sheet name="Hard" sheetId="14" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="23">
   <si>
     <t>Outcome</t>
   </si>
@@ -18806,8 +18806,8 @@
       <c r="J1">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
-        <v>2</v>
+      <c r="K1">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -19519,35 +19519,35 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f>B13</f>
+        <f t="shared" ref="B3:B8" si="0">B13</f>
         <v>0.35360813639536137</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3" si="0">C13</f>
+        <f t="shared" ref="C3" si="1">C13</f>
         <v>0.3738748853821432</v>
       </c>
       <c r="D3">
-        <f>D13</f>
+        <f t="shared" ref="D3:I8" si="2">D13</f>
         <v>0.39446844550254284</v>
       </c>
       <c r="E3">
-        <f>E13</f>
+        <f t="shared" si="2"/>
         <v>0.41640366958226238</v>
       </c>
       <c r="F3">
-        <f>F13</f>
+        <f t="shared" si="2"/>
         <v>0.42315049208499783</v>
       </c>
       <c r="G3">
-        <f>G13</f>
+        <f t="shared" si="2"/>
         <v>0.26231240836153336</v>
       </c>
       <c r="H3">
-        <f>H13</f>
+        <f t="shared" si="2"/>
         <v>0.2447412422511914</v>
       </c>
       <c r="I3">
-        <f>I13</f>
+        <f t="shared" si="2"/>
         <v>0.2284251594344453</v>
       </c>
       <c r="J3">
@@ -19564,7 +19564,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <f>B14</f>
+        <f t="shared" si="0"/>
         <v>0.13980913952773527</v>
       </c>
       <c r="C4">
@@ -19572,27 +19572,27 @@
         <v>0.13503398781113993</v>
       </c>
       <c r="D4">
-        <f>D14</f>
+        <f t="shared" si="2"/>
         <v>0.13048973584959825</v>
       </c>
       <c r="E4">
-        <f>E14</f>
+        <f t="shared" si="2"/>
         <v>0.12225128527055079</v>
       </c>
       <c r="F4">
-        <f>F14</f>
+        <f t="shared" si="2"/>
         <v>0.16543817650334638</v>
       </c>
       <c r="G4">
-        <f>G14</f>
+        <f t="shared" si="2"/>
         <v>0.36856619379423861</v>
       </c>
       <c r="H4">
-        <f>H14</f>
+        <f t="shared" si="2"/>
         <v>0.12856654444917001</v>
       </c>
       <c r="I4">
-        <f>I14</f>
+        <f t="shared" si="2"/>
         <v>0.119995441485892</v>
       </c>
       <c r="J4">
@@ -19609,7 +19609,7 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <f>B15</f>
+        <f t="shared" si="0"/>
         <v>0.13490735037469442</v>
       </c>
       <c r="C5">
@@ -19617,27 +19617,27 @@
         <v>0.13048232645474483</v>
       </c>
       <c r="D5">
-        <f>D15</f>
+        <f t="shared" si="2"/>
         <v>0.12593807449320316</v>
       </c>
       <c r="E5">
-        <f>E15</f>
+        <f t="shared" si="2"/>
         <v>0.12225128527055079</v>
       </c>
       <c r="F5">
-        <f>F15</f>
+        <f t="shared" si="2"/>
         <v>0.10626657887021028</v>
       </c>
       <c r="G5">
-        <f>G15</f>
+        <f t="shared" si="2"/>
         <v>0.13779696302500785</v>
       </c>
       <c r="H5">
-        <f>H15</f>
+        <f t="shared" si="2"/>
         <v>0.35933577521840082</v>
       </c>
       <c r="I5">
-        <f>I15</f>
+        <f t="shared" si="2"/>
         <v>0.119995441485892</v>
       </c>
       <c r="J5">
@@ -19654,7 +19654,7 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <f>B16</f>
+        <f t="shared" si="0"/>
         <v>0.12965543342500779</v>
       </c>
       <c r="C6">
@@ -19662,27 +19662,27 @@
         <v>0.12558053730170399</v>
       </c>
       <c r="D6">
-        <f>D16</f>
+        <f t="shared" si="2"/>
         <v>0.12138641313680808</v>
       </c>
       <c r="E6">
-        <f>E16</f>
+        <f t="shared" si="2"/>
         <v>0.11769962391415568</v>
       </c>
       <c r="F6">
-        <f>F16</f>
+        <f t="shared" si="2"/>
         <v>0.10626657887021028</v>
       </c>
       <c r="G6">
-        <f>G16</f>
+        <f t="shared" si="2"/>
         <v>7.8625365391871746E-2</v>
       </c>
       <c r="H6">
-        <f>H16</f>
+        <f t="shared" si="2"/>
         <v>0.12856654444917001</v>
       </c>
       <c r="I6">
-        <f>I16</f>
+        <f t="shared" si="2"/>
         <v>0.35076467225512281</v>
       </c>
       <c r="J6">
@@ -19699,7 +19699,7 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <f>B17</f>
+        <f t="shared" si="0"/>
         <v>0.12402645577124111</v>
       </c>
       <c r="C7">
@@ -19707,27 +19707,27 @@
         <v>0.12032862035201736</v>
       </c>
       <c r="D7">
-        <f>D17</f>
+        <f t="shared" si="2"/>
         <v>0.1164846239837672</v>
       </c>
       <c r="E7">
-        <f>E17</f>
+        <f t="shared" si="2"/>
         <v>0.11314796255776062</v>
       </c>
       <c r="F7">
-        <f>F17</f>
+        <f t="shared" si="2"/>
         <v>0.1017149175138152</v>
       </c>
       <c r="G7">
-        <f>G17</f>
+        <f t="shared" si="2"/>
         <v>7.8625365391871746E-2</v>
       </c>
       <c r="H7">
-        <f>H17</f>
+        <f t="shared" si="2"/>
         <v>6.9394946816033906E-2</v>
       </c>
       <c r="I7">
-        <f>I17</f>
+        <f t="shared" si="2"/>
         <v>0.119995441485892</v>
       </c>
       <c r="J7">
@@ -19744,7 +19744,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="4">
-        <f>B18</f>
+        <f t="shared" si="0"/>
         <v>0.11799348450596003</v>
       </c>
       <c r="C8" s="4">
@@ -19752,27 +19752,27 @@
         <v>0.11469964269825066</v>
       </c>
       <c r="D8" s="4">
-        <f>D18</f>
+        <f t="shared" si="2"/>
         <v>0.11123270703408056</v>
       </c>
       <c r="E8" s="4">
-        <f>E18</f>
+        <f t="shared" si="2"/>
         <v>0.10824617340471974</v>
       </c>
       <c r="F8" s="4">
-        <f>F18</f>
+        <f t="shared" si="2"/>
         <v>9.7163256157420108E-2</v>
       </c>
       <c r="G8" s="4">
-        <f>G18</f>
+        <f t="shared" si="2"/>
         <v>7.4073704035476667E-2</v>
       </c>
       <c r="H8" s="4">
-        <f>H18</f>
+        <f t="shared" si="2"/>
         <v>6.9394946816033906E-2</v>
       </c>
       <c r="I8" s="4">
-        <f>I18</f>
+        <f t="shared" si="2"/>
         <v>6.0823843852755917E-2</v>
       </c>
       <c r="J8" s="4">
@@ -19793,39 +19793,39 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:K9" si="1">SUM(C3:C8)</f>
+        <f t="shared" ref="C9:K9" si="3">SUM(C3:C8)</f>
         <v>0.99999999999999989</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19875,178 +19875,178 @@
         <v>11</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" ref="L12:AE12" si="2">K12+1</f>
+        <f t="shared" ref="L12:AE12" si="4">K12+1</f>
         <v>12</v>
       </c>
       <c r="M12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="O12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="P12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="Q12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="R12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="S12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="T12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="U12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="V12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="W12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="X12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="Y12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="Z12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="AA12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="AB12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="AC12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="AD12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="AE12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="AG12" s="4">
         <v>12</v>
       </c>
       <c r="AH12" s="4">
-        <f t="shared" ref="AH12:BH12" si="3">AG12+1</f>
+        <f t="shared" ref="AH12:BH12" si="5">AG12+1</f>
         <v>13</v>
       </c>
       <c r="AI12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="AJ12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="AK12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="AL12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="AM12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="AN12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="AO12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="AP12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="AQ12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="AR12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="AS12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="AT12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="AU12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="AV12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="AW12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="AX12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="AY12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="AZ12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="BE12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="BF12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="BG12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="BH12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
     </row>
@@ -20169,35 +20169,35 @@
         <v>0.48267271400214928</v>
       </c>
       <c r="AR13">
-        <f t="shared" ref="AR13:AR18" si="4">M13</f>
+        <f t="shared" ref="AR13:AR18" si="6">M13</f>
         <v>0.51962466300199572</v>
       </c>
       <c r="AS13">
-        <f t="shared" ref="AS13:AS18" si="5">N13</f>
+        <f t="shared" ref="AS13:AS18" si="7">N13</f>
         <v>0.55393718707328177</v>
       </c>
       <c r="AT13">
-        <f t="shared" ref="AT13:AT18" si="6">O13</f>
+        <f t="shared" ref="AT13:AT18" si="8">O13</f>
         <v>0.58579881656804733</v>
       </c>
       <c r="AU13">
-        <f t="shared" ref="AU13:AU18" si="7">P13</f>
+        <f t="shared" ref="AU13:AU18" si="9">P13</f>
         <v>0.61538461538461542</v>
       </c>
       <c r="AV13">
-        <f t="shared" ref="AV13:AV18" si="8">Q13</f>
+        <f t="shared" ref="AV13:AV18" si="10">Q13</f>
         <v>0</v>
       </c>
       <c r="AW13">
-        <f t="shared" ref="AW13:AW18" si="9">R13</f>
+        <f t="shared" ref="AW13:AW18" si="11">R13</f>
         <v>0</v>
       </c>
       <c r="AX13">
-        <f t="shared" ref="AX13:AX18" si="10">S13</f>
+        <f t="shared" ref="AX13:AX18" si="12">S13</f>
         <v>0</v>
       </c>
       <c r="AY13">
-        <f t="shared" ref="AY13:AY18" si="11">T13</f>
+        <f t="shared" ref="AY13:AY18" si="13">T13</f>
         <v>0</v>
       </c>
       <c r="AZ13">
@@ -20296,43 +20296,43 @@
         <v>1</v>
       </c>
       <c r="AQ14">
-        <f t="shared" ref="AQ14:AQ18" si="12">L14</f>
+        <f t="shared" ref="AQ14:AQ18" si="14">L14</f>
         <v>0.10346545719957015</v>
       </c>
       <c r="AR14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.6075067399600853E-2</v>
       </c>
       <c r="AS14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.9212562585343644E-2</v>
       </c>
       <c r="AT14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8.2840236686390525E-2</v>
       </c>
       <c r="AU14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="AV14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AW14">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AX14">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AY14">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="AX14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AY14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
       <c r="AZ14">
-        <f t="shared" ref="AZ13:AZ18" si="13">U14</f>
+        <f t="shared" ref="AZ14:AZ18" si="15">U14</f>
         <v>0</v>
       </c>
     </row>
@@ -20427,43 +20427,43 @@
         <v>1</v>
       </c>
       <c r="AQ15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.10346545719957015</v>
       </c>
       <c r="AR15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.6075067399600853E-2</v>
       </c>
       <c r="AS15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.9212562585343644E-2</v>
       </c>
       <c r="AT15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8.2840236686390525E-2</v>
       </c>
       <c r="AU15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="AV15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AW15">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AX15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
+      <c r="AW15">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AX15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
       <c r="AY15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AZ15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -20558,43 +20558,43 @@
         <v>1</v>
       </c>
       <c r="AQ16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.10346545719957015</v>
       </c>
       <c r="AR16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.6075067399600853E-2</v>
       </c>
       <c r="AS16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.9212562585343644E-2</v>
       </c>
       <c r="AT16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8.2840236686390525E-2</v>
       </c>
       <c r="AU16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="AV16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AW16">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AX16">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AY16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="AX16">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AY16">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
       <c r="AZ16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -20689,43 +20689,43 @@
         <v>1</v>
       </c>
       <c r="AQ17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.10346545719957015</v>
       </c>
       <c r="AR17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.6075067399600853E-2</v>
       </c>
       <c r="AS17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.9212562585343644E-2</v>
       </c>
       <c r="AT17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8.2840236686390525E-2</v>
       </c>
       <c r="AU17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="AV17">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AW17">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AX17">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
+      <c r="AW17">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AX17">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
       <c r="AY17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AZ17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -20838,43 +20838,43 @@
         <v>1</v>
       </c>
       <c r="AQ18" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.10346545719957015</v>
       </c>
       <c r="AR18" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.6075067399600853E-2</v>
       </c>
       <c r="AS18" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8.9212562585343644E-2</v>
       </c>
       <c r="AT18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8.2840236686390525E-2</v>
       </c>
       <c r="AU18" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="AV18" s="4">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AW18" s="4">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AX18" s="4">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AY18" s="4">
+      <c r="AW18" s="4">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="AX18" s="4">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AY18" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
       <c r="AZ18" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -20887,199 +20887,199 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:AZ19" si="14">SUM(C13:C18)</f>
+        <f t="shared" ref="C19:AZ19" si="16">SUM(C13:C18)</f>
         <v>0.99999999999999989</v>
       </c>
       <c r="D19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="E19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="F19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="G19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="H19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="I19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="J19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="K19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="L19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="M19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="N19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="O19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="P19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="R19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="S19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="T19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="U19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="V19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="W19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="X19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AB19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AC19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AD19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AE19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AG19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="AH19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="AI19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="AJ19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="AK19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AL19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AM19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AN19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AO19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AP19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AQ19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="AR19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="AS19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="AT19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="AU19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="AV19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AW19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AX19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AY19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="AZ19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: made EV calculations based on deck composition
</commit_message>
<xml_diff>
--- a/src/main/resources/strategies/CustomCardCounting.xlsx
+++ b/src/main/resources/strategies/CustomCardCounting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\BlackjackSimulator\src\main\resources\strategies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\IdeaProjects\BlackjackSimulator\src\main\resources\strategies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C4BF01-8F90-4A4D-BF28-32D0FEE8826A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D71356-C94E-4EE2-A0B1-E1DF82662E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1452" windowWidth="28800" windowHeight="15828" xr2:uid="{21CDB781-D789-4925-8E21-207DEAF49322}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{21CDB781-D789-4925-8E21-207DEAF49322}"/>
   </bookViews>
   <sheets>
     <sheet name="Hard" sheetId="14" r:id="rId1"/>
@@ -7193,9 +7193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -10856,8 +10854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12365,9 +12363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:M92"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -12411,43 +12407,43 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <f>$B77*(1/13)</f>
+        <f>$B77*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:I2" si="0">$B77*(1/13)</f>
+        <f>$B77*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="D2">
-        <f t="shared" si="0"/>
+        <f>$B77*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="E2">
-        <f t="shared" si="0"/>
+        <f>$B77*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="F2">
-        <f t="shared" si="0"/>
+        <f>$B77*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="G2">
-        <f t="shared" si="0"/>
+        <f>$B77*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="H2">
-        <f t="shared" si="0"/>
+        <f>$B77*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="I2">
-        <f t="shared" si="0"/>
+        <f>$B77*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="J2">
-        <f>$B77*(4/13)*(12/13)</f>
+        <f>$B77*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.3612268477994475E-3</v>
       </c>
       <c r="K2">
-        <f>$B77*(1/13)*(9/13)</f>
+        <f>$B77*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3023003396239633E-4</v>
       </c>
     </row>
@@ -12457,641 +12453,641 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:I3" ca="1" si="1">$B78*(1/13)</f>
+        <f ca="1">$B78*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="C3">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">$B78*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="D3">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">$B78*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="E3">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">$B78*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="F3">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">$B78*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="G3">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">$B78*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="H3">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">$B78*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="I3">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">$B78*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J16" ca="1" si="2">$B78*(4/13)*(12/13)</f>
+        <f ca="1">$B78*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.3612268477994475E-3</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K16" ca="1" si="3">$B78*(1/13)*(9/13)</f>
+        <f ca="1">$B78*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3023003396239633E-4</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A40" si="4">A3+1</f>
+        <f t="shared" ref="A4:A40" si="0">A3+1</f>
         <v>7</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:I4" ca="1" si="5">$B79*(1/13)</f>
+        <f ca="1">$B79*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="C4">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">$B79*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="D4">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">$B79*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="E4">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">$B79*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="F4">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">$B79*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="G4">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">$B79*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="H4">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">$B79*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="I4">
-        <f t="shared" ca="1" si="5"/>
+        <f ca="1">$B79*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="J4">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">$B79*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>6.7224536955988951E-3</v>
       </c>
       <c r="K4">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">$B79*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.2604600679247927E-3</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:I5" ca="1" si="6">$B80*(1/13)</f>
+        <f ca="1">$B80*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="C5">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">$B80*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="D5">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">$B80*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="E5">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">$B80*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="F5">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">$B80*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="G5">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">$B80*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="H5">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">$B80*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="I5">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">$B80*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8206645425580339E-3</v>
       </c>
       <c r="J5">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">$B80*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>6.7224536955988951E-3</v>
       </c>
       <c r="K5">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">$B80*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.2604600679247927E-3</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:I6" ca="1" si="7">$B81*(1/13)</f>
+        <f ca="1">$B81*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="7"/>
+        <f ca="1">$B81*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="D6">
-        <f t="shared" ca="1" si="7"/>
+        <f ca="1">$B81*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="E6">
-        <f t="shared" ca="1" si="7"/>
+        <f ca="1">$B81*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="F6">
-        <f t="shared" ca="1" si="7"/>
+        <f ca="1">$B81*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="G6">
-        <f t="shared" ca="1" si="7"/>
+        <f ca="1">$B81*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="H6">
-        <f t="shared" ca="1" si="7"/>
+        <f ca="1">$B81*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="I6">
-        <f t="shared" ca="1" si="7"/>
+        <f ca="1">$B81*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="J6">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">$B81*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.0083680543398345E-2</v>
       </c>
       <c r="K6">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">$B81*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8906901018871894E-3</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7:I7" ca="1" si="8">$B82*(1/13)</f>
+        <f ca="1">$B82*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="8"/>
+        <f ca="1">$B82*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="D7">
-        <f t="shared" ca="1" si="8"/>
+        <f ca="1">$B82*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="E7">
-        <f t="shared" ca="1" si="8"/>
+        <f ca="1">$B82*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="F7">
-        <f t="shared" ca="1" si="8"/>
+        <f ca="1">$B82*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="G7">
-        <f t="shared" ca="1" si="8"/>
+        <f ca="1">$B82*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="H7">
-        <f t="shared" ca="1" si="8"/>
+        <f ca="1">$B82*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="I7">
-        <f t="shared" ca="1" si="8"/>
+        <f ca="1">$B82*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>2.7309968138370514E-3</v>
       </c>
       <c r="J7">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">$B82*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.0083680543398345E-2</v>
       </c>
       <c r="K7">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">$B82*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.8906901018871894E-3</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B8:I8" ca="1" si="9">$B83*(1/13)</f>
+        <f ca="1">$B83*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160687E-3</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="9"/>
+        <f ca="1">$B83*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160687E-3</v>
       </c>
       <c r="D8">
-        <f t="shared" ca="1" si="9"/>
+        <f ca="1">$B83*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160687E-3</v>
       </c>
       <c r="E8">
-        <f t="shared" ca="1" si="9"/>
+        <f ca="1">$B83*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160687E-3</v>
       </c>
       <c r="F8">
-        <f t="shared" ca="1" si="9"/>
+        <f ca="1">$B83*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160687E-3</v>
       </c>
       <c r="G8">
-        <f t="shared" ca="1" si="9"/>
+        <f ca="1">$B83*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160687E-3</v>
       </c>
       <c r="H8">
-        <f t="shared" ca="1" si="9"/>
+        <f ca="1">$B83*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160687E-3</v>
       </c>
       <c r="I8">
-        <f t="shared" ca="1" si="9"/>
+        <f ca="1">$B83*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160687E-3</v>
       </c>
       <c r="J8">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">$B83*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.3444907391197794E-2</v>
       </c>
       <c r="K8">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">$B83*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>2.5209201358495858E-3</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9:I9" ca="1" si="10">$B84*(1/13)</f>
+        <f ca="1">$B84*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="C9">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">$B84*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="D9">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">$B84*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="E9">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">$B84*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="F9">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">$B84*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="G9">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">$B84*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="H9">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">$B84*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="I9">
-        <f t="shared" ca="1" si="10"/>
+        <f ca="1">$B84*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="J9">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">$B84*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>2.3528587934596137E-2</v>
       </c>
       <c r="K9">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">$B84*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>4.4116102377367754E-3</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B10">
-        <f t="shared" ref="B10:I10" ca="1" si="11">$B85*(1/13)</f>
+        <f ca="1">$B85*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="C10">
-        <f t="shared" ca="1" si="11"/>
+        <f ca="1">$B85*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="D10">
-        <f t="shared" ca="1" si="11"/>
+        <f ca="1">$B85*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="E10">
-        <f t="shared" ca="1" si="11"/>
+        <f ca="1">$B85*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="F10">
-        <f t="shared" ca="1" si="11"/>
+        <f ca="1">$B85*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="G10">
-        <f t="shared" ca="1" si="11"/>
+        <f ca="1">$B85*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="H10">
-        <f t="shared" ca="1" si="11"/>
+        <f ca="1">$B85*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="I10">
-        <f t="shared" ca="1" si="11"/>
+        <f ca="1">$B85*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3723258989531201E-3</v>
       </c>
       <c r="J10">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">$B85*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>2.3528587934596137E-2</v>
       </c>
       <c r="K10">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">$B85*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>4.4116102377367754E-3</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B11">
-        <f t="shared" ref="B11:I11" ca="1" si="12">$B86*(1/13)</f>
+        <f ca="1">$B86*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="C11">
-        <f t="shared" ca="1" si="12"/>
+        <f ca="1">$B86*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="D11">
-        <f t="shared" ca="1" si="12"/>
+        <f ca="1">$B86*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="E11">
-        <f t="shared" ca="1" si="12"/>
+        <f ca="1">$B86*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="F11">
-        <f t="shared" ca="1" si="12"/>
+        <f ca="1">$B86*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="G11">
-        <f t="shared" ca="1" si="12"/>
+        <f ca="1">$B86*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="H11">
-        <f t="shared" ca="1" si="12"/>
+        <f ca="1">$B86*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="I11">
-        <f t="shared" ca="1" si="12"/>
+        <f ca="1">$B86*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="J11">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">$B86*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>2.016736108679669E-2</v>
       </c>
       <c r="K11">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">$B86*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.7813802037743789E-3</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B12">
-        <f t="shared" ref="B12:I12" ca="1" si="13">$B87*(1/13)</f>
+        <f ca="1">$B87*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="C12">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1">$B87*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="D12">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1">$B87*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="E12">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1">$B87*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="F12">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1">$B87*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="G12">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1">$B87*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="H12">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1">$B87*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="I12">
-        <f t="shared" ca="1" si="13"/>
+        <f ca="1">$B87*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>5.4619936276741029E-3</v>
       </c>
       <c r="J12">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">$B87*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>2.016736108679669E-2</v>
       </c>
       <c r="K12">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">$B87*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.7813802037743789E-3</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B13">
-        <f t="shared" ref="B13:I13" ca="1" si="14">$B88*(1/13)</f>
+        <f ca="1">$B88*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="C13">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1">$B88*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="D13">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1">$B88*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="E13">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1">$B88*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="F13">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1">$B88*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="G13">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1">$B88*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="H13">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1">$B88*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="I13">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1">$B88*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="J13">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">$B88*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.6806134238997239E-2</v>
       </c>
       <c r="K13">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">$B88*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.1511501698119823E-3</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14:I14" ca="1" si="15">$B89*(1/13)</f>
+        <f ca="1">$B89*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="C14">
-        <f t="shared" ca="1" si="15"/>
+        <f ca="1">$B89*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="D14">
-        <f t="shared" ca="1" si="15"/>
+        <f ca="1">$B89*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="E14">
-        <f t="shared" ca="1" si="15"/>
+        <f ca="1">$B89*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="F14">
-        <f t="shared" ca="1" si="15"/>
+        <f ca="1">$B89*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="G14">
-        <f t="shared" ca="1" si="15"/>
+        <f ca="1">$B89*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="H14">
-        <f t="shared" ca="1" si="15"/>
+        <f ca="1">$B89*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="I14">
-        <f t="shared" ca="1" si="15"/>
+        <f ca="1">$B89*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950856E-3</v>
       </c>
       <c r="J14">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">$B89*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.6806134238997239E-2</v>
       </c>
       <c r="K14">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">$B89*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.1511501698119823E-3</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B15">
-        <f t="shared" ref="B15:I15" ca="1" si="16">$B90*(1/13)</f>
+        <f ca="1">$B90*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="C15">
-        <f t="shared" ca="1" si="16"/>
+        <f ca="1">$B90*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="D15">
-        <f t="shared" ca="1" si="16"/>
+        <f ca="1">$B90*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="E15">
-        <f t="shared" ca="1" si="16"/>
+        <f ca="1">$B90*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="F15">
-        <f t="shared" ca="1" si="16"/>
+        <f ca="1">$B90*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="G15">
-        <f t="shared" ca="1" si="16"/>
+        <f ca="1">$B90*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="H15">
-        <f t="shared" ca="1" si="16"/>
+        <f ca="1">$B90*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="I15">
-        <f t="shared" ca="1" si="16"/>
+        <f ca="1">$B90*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="J15">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">$B90*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.344490739119779E-2</v>
       </c>
       <c r="K15">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">$B90*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>2.5209201358495853E-3</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:I16" ca="1" si="17">$B91*(1/13)</f>
+        <f ca="1">$B91*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="C16">
-        <f t="shared" ca="1" si="17"/>
+        <f ca="1">$B91*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="D16">
-        <f t="shared" ca="1" si="17"/>
+        <f ca="1">$B91*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="E16">
-        <f t="shared" ca="1" si="17"/>
+        <f ca="1">$B91*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="F16">
-        <f t="shared" ca="1" si="17"/>
+        <f ca="1">$B91*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="G16">
-        <f t="shared" ca="1" si="17"/>
+        <f ca="1">$B91*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="H16">
-        <f t="shared" ca="1" si="17"/>
+        <f ca="1">$B91*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="I16">
-        <f t="shared" ca="1" si="17"/>
+        <f ca="1">$B91*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="J16">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">$B91*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.344490739119779E-2</v>
       </c>
       <c r="K16">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">$B91*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>2.5209201358495853E-3</v>
       </c>
       <c r="M16">
@@ -13109,411 +13105,411 @@
         <v>13</v>
       </c>
       <c r="B21">
-        <f>2*(1/13)^3</f>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B6/SUM(Deck!$B$5:$B$14))*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:I28" si="18">2*(1/13)^3</f>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B6/SUM(Deck!$B$5:$B$14))*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="D21">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B6/SUM(Deck!$B$5:$B$14))*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="E21">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B6/SUM(Deck!$B$5:$B$14))*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="F21">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B6/SUM(Deck!$B$5:$B$14))*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="G21">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B6/SUM(Deck!$B$5:$B$14))*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="H21">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B6/SUM(Deck!$B$5:$B$14))*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="I21">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B6/SUM(Deck!$B$5:$B$14))*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="J21">
-        <f>2*(1/13)^2*(4/13)*(12/13)</f>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B6/SUM(Deck!$B$5:$B$14))*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.3612268477994475E-3</v>
       </c>
       <c r="K21">
-        <f>2*(1/13)^3*(9/13)</f>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B6/SUM(Deck!$B$5:$B$14))*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3023003396239633E-4</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22:B28" si="19">2*(1/13)^3</f>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B7/SUM(Deck!$B$5:$B$14))*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="C22">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B7/SUM(Deck!$B$5:$B$14))*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="D22">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B7/SUM(Deck!$B$5:$B$14))*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="E22">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B7/SUM(Deck!$B$5:$B$14))*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="F22">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B7/SUM(Deck!$B$5:$B$14))*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="G22">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B7/SUM(Deck!$B$5:$B$14))*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="H22">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B7/SUM(Deck!$B$5:$B$14))*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="I22">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B7/SUM(Deck!$B$5:$B$14))*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="J22">
-        <f t="shared" ref="J22:J28" si="20">2*(1/13)^2*(4/13)*(12/13)</f>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B7/SUM(Deck!$B$5:$B$14))*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.3612268477994475E-3</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22:K28" si="21">2*(1/13)^3*(9/13)</f>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B7/SUM(Deck!$B$5:$B$14))*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3023003396239633E-4</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B23">
-        <f t="shared" si="19"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B8/SUM(Deck!$B$5:$B$14))*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="C23">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B8/SUM(Deck!$B$5:$B$14))*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="D23">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B8/SUM(Deck!$B$5:$B$14))*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="E23">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B8/SUM(Deck!$B$5:$B$14))*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="F23">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B8/SUM(Deck!$B$5:$B$14))*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="G23">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B8/SUM(Deck!$B$5:$B$14))*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="H23">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B8/SUM(Deck!$B$5:$B$14))*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="I23">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B8/SUM(Deck!$B$5:$B$14))*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="J23">
-        <f t="shared" si="20"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B8/SUM(Deck!$B$5:$B$14))*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.3612268477994475E-3</v>
       </c>
       <c r="K23">
-        <f t="shared" si="21"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B8/SUM(Deck!$B$5:$B$14))*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3023003396239633E-4</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B24">
-        <f t="shared" si="19"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B9/SUM(Deck!$B$5:$B$14))*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="C24">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B9/SUM(Deck!$B$5:$B$14))*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="D24">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B9/SUM(Deck!$B$5:$B$14))*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="E24">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B9/SUM(Deck!$B$5:$B$14))*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="F24">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B9/SUM(Deck!$B$5:$B$14))*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="G24">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B9/SUM(Deck!$B$5:$B$14))*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="H24">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B9/SUM(Deck!$B$5:$B$14))*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="I24">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B9/SUM(Deck!$B$5:$B$14))*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="J24">
-        <f t="shared" si="20"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B9/SUM(Deck!$B$5:$B$14))*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.3612268477994475E-3</v>
       </c>
       <c r="K24">
-        <f t="shared" si="21"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B9/SUM(Deck!$B$5:$B$14))*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3023003396239633E-4</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B25">
-        <f t="shared" si="19"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B10/SUM(Deck!$B$5:$B$14))*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="C25">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B10/SUM(Deck!$B$5:$B$14))*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="D25">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B10/SUM(Deck!$B$5:$B$14))*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="E25">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B10/SUM(Deck!$B$5:$B$14))*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="F25">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B10/SUM(Deck!$B$5:$B$14))*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="G25">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B10/SUM(Deck!$B$5:$B$14))*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="H25">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B10/SUM(Deck!$B$5:$B$14))*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="I25">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B10/SUM(Deck!$B$5:$B$14))*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="J25">
-        <f t="shared" si="20"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B10/SUM(Deck!$B$5:$B$14))*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.3612268477994475E-3</v>
       </c>
       <c r="K25">
-        <f t="shared" si="21"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B10/SUM(Deck!$B$5:$B$14))*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3023003396239633E-4</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B26">
-        <f t="shared" si="19"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B11/SUM(Deck!$B$5:$B$14))*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="C26">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B11/SUM(Deck!$B$5:$B$14))*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="D26">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B11/SUM(Deck!$B$5:$B$14))*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="E26">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B11/SUM(Deck!$B$5:$B$14))*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="F26">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B11/SUM(Deck!$B$5:$B$14))*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="G26">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B11/SUM(Deck!$B$5:$B$14))*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="H26">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B11/SUM(Deck!$B$5:$B$14))*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="I26">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B11/SUM(Deck!$B$5:$B$14))*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="J26">
-        <f t="shared" si="20"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B11/SUM(Deck!$B$5:$B$14))*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.3612268477994475E-3</v>
       </c>
       <c r="K26">
-        <f t="shared" si="21"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B11/SUM(Deck!$B$5:$B$14))*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3023003396239633E-4</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B27">
-        <f t="shared" si="19"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B12/SUM(Deck!$B$5:$B$14))*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="C27">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B12/SUM(Deck!$B$5:$B$14))*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="D27">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B12/SUM(Deck!$B$5:$B$14))*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="E27">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B12/SUM(Deck!$B$5:$B$14))*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="F27">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B12/SUM(Deck!$B$5:$B$14))*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="G27">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B12/SUM(Deck!$B$5:$B$14))*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="H27">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B12/SUM(Deck!$B$5:$B$14))*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="I27">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B12/SUM(Deck!$B$5:$B$14))*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="J27">
-        <f t="shared" si="20"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B12/SUM(Deck!$B$5:$B$14))*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.3612268477994475E-3</v>
       </c>
       <c r="K27">
-        <f t="shared" si="21"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B12/SUM(Deck!$B$5:$B$14))*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3023003396239633E-4</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B28">
-        <f t="shared" si="19"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B13/SUM(Deck!$B$5:$B$14))*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="C28">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B13/SUM(Deck!$B$5:$B$14))*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="D28">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B13/SUM(Deck!$B$5:$B$14))*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="E28">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B13/SUM(Deck!$B$5:$B$14))*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="F28">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B13/SUM(Deck!$B$5:$B$14))*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="G28">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B13/SUM(Deck!$B$5:$B$14))*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="H28">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B13/SUM(Deck!$B$5:$B$14))*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="I28">
-        <f t="shared" si="18"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B13/SUM(Deck!$B$5:$B$14))*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>9.1033227127901696E-4</v>
       </c>
       <c r="J28">
-        <f t="shared" si="20"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B13/SUM(Deck!$B$5:$B$14))*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.3612268477994475E-3</v>
       </c>
       <c r="K28">
-        <f t="shared" si="21"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B13/SUM(Deck!$B$5:$B$14))*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>6.3023003396239633E-4</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B29">
-        <f>2*(1/13)^2*(4/13)</f>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B14/SUM(Deck!$B$5:$B$14))*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="C29">
-        <f t="shared" ref="C29:I29" si="22">2*(1/13)^2*(4/13)</f>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B14/SUM(Deck!$B$5:$B$14))*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="D29">
-        <f t="shared" si="22"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B14/SUM(Deck!$B$5:$B$14))*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="E29">
-        <f t="shared" si="22"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B14/SUM(Deck!$B$5:$B$14))*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="F29">
-        <f t="shared" si="22"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B14/SUM(Deck!$B$5:$B$14))*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="G29">
-        <f t="shared" si="22"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B14/SUM(Deck!$B$5:$B$14))*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="H29">
-        <f t="shared" si="22"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B14/SUM(Deck!$B$5:$B$14))*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="I29">
-        <f t="shared" si="22"/>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B14/SUM(Deck!$B$5:$B$14))*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>3.6413290851160678E-3</v>
       </c>
       <c r="J29">
-        <f>2*(1/13)*(4/13)*(4/13)*(12/13)</f>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B14/SUM(Deck!$B$5:$B$14))*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.344490739119779E-2</v>
       </c>
       <c r="K29">
-        <f>2*(1/13)*(4/13)*(1/13)*(9/13)</f>
+        <f>2*(Deck!$B$2/SUM(Deck!$B$2:$K$2))*(Deck!$B14/SUM(Deck!$B$5:$B$14))*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>2.5209201358495853E-3</v>
       </c>
     </row>
@@ -13527,411 +13523,411 @@
         <v>2</v>
       </c>
       <c r="B32">
-        <f>(1/13)^3</f>
+        <f>(Deck!$B6/SUM(Deck!$B$5:$B$14))^2*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="C32">
-        <f t="shared" ref="C32:I39" si="23">(1/13)^3</f>
+        <f>(Deck!$B6/SUM(Deck!$B$5:$B$14))^2*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="D32">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B6/SUM(Deck!$B$5:$B$14))^2*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="E32">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B6/SUM(Deck!$B$5:$B$14))^2*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="F32">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B6/SUM(Deck!$B$5:$B$14))^2*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="G32">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B6/SUM(Deck!$B$5:$B$14))^2*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="H32">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B6/SUM(Deck!$B$5:$B$14))^2*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="I32">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B6/SUM(Deck!$B$5:$B$14))^2*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="J32">
-        <f>(1/13)^2*(4/13)*(12/13)</f>
+        <f>(Deck!$B6/SUM(Deck!$B$5:$B$14))^2*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.6806134238997238E-3</v>
       </c>
       <c r="K32">
-        <f>(1/13)^3*(9/13)</f>
+        <f>(Deck!$B6/SUM(Deck!$B$5:$B$14))^2*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.1511501698119817E-4</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B33">
-        <f t="shared" ref="B33:B39" si="24">(1/13)^3</f>
+        <f>(Deck!$B7/SUM(Deck!$B$5:$B$14))^2*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="C33">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B7/SUM(Deck!$B$5:$B$14))^2*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="D33">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B7/SUM(Deck!$B$5:$B$14))^2*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="E33">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B7/SUM(Deck!$B$5:$B$14))^2*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="F33">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B7/SUM(Deck!$B$5:$B$14))^2*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="G33">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B7/SUM(Deck!$B$5:$B$14))^2*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="H33">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B7/SUM(Deck!$B$5:$B$14))^2*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="I33">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B7/SUM(Deck!$B$5:$B$14))^2*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="J33">
-        <f t="shared" ref="J33:J39" si="25">(1/13)^2*(4/13)*(12/13)</f>
+        <f>(Deck!$B7/SUM(Deck!$B$5:$B$14))^2*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.6806134238997238E-3</v>
       </c>
       <c r="K33">
-        <f t="shared" ref="K33:K39" si="26">(1/13)^3*(9/13)</f>
+        <f>(Deck!$B7/SUM(Deck!$B$5:$B$14))^2*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.1511501698119817E-4</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B34">
-        <f t="shared" si="24"/>
+        <f>(Deck!$B8/SUM(Deck!$B$5:$B$14))^2*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="C34">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B8/SUM(Deck!$B$5:$B$14))^2*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="D34">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B8/SUM(Deck!$B$5:$B$14))^2*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="E34">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B8/SUM(Deck!$B$5:$B$14))^2*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="F34">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B8/SUM(Deck!$B$5:$B$14))^2*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="G34">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B8/SUM(Deck!$B$5:$B$14))^2*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="H34">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B8/SUM(Deck!$B$5:$B$14))^2*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="I34">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B8/SUM(Deck!$B$5:$B$14))^2*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="J34">
-        <f t="shared" si="25"/>
+        <f>(Deck!$B8/SUM(Deck!$B$5:$B$14))^2*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.6806134238997238E-3</v>
       </c>
       <c r="K34">
-        <f t="shared" si="26"/>
+        <f>(Deck!$B8/SUM(Deck!$B$5:$B$14))^2*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.1511501698119817E-4</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B35">
-        <f t="shared" si="24"/>
+        <f>(Deck!$B9/SUM(Deck!$B$5:$B$14))^2*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="C35">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B9/SUM(Deck!$B$5:$B$14))^2*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="D35">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B9/SUM(Deck!$B$5:$B$14))^2*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="E35">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B9/SUM(Deck!$B$5:$B$14))^2*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="F35">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B9/SUM(Deck!$B$5:$B$14))^2*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="G35">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B9/SUM(Deck!$B$5:$B$14))^2*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="H35">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B9/SUM(Deck!$B$5:$B$14))^2*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="I35">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B9/SUM(Deck!$B$5:$B$14))^2*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="J35">
-        <f t="shared" si="25"/>
+        <f>(Deck!$B9/SUM(Deck!$B$5:$B$14))^2*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.6806134238997238E-3</v>
       </c>
       <c r="K35">
-        <f t="shared" si="26"/>
+        <f>(Deck!$B9/SUM(Deck!$B$5:$B$14))^2*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.1511501698119817E-4</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B36">
-        <f t="shared" si="24"/>
+        <f>(Deck!$B10/SUM(Deck!$B$5:$B$14))^2*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="C36">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B10/SUM(Deck!$B$5:$B$14))^2*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="D36">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B10/SUM(Deck!$B$5:$B$14))^2*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="E36">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B10/SUM(Deck!$B$5:$B$14))^2*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="F36">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B10/SUM(Deck!$B$5:$B$14))^2*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="G36">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B10/SUM(Deck!$B$5:$B$14))^2*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="H36">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B10/SUM(Deck!$B$5:$B$14))^2*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="I36">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B10/SUM(Deck!$B$5:$B$14))^2*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="J36">
-        <f t="shared" si="25"/>
+        <f>(Deck!$B10/SUM(Deck!$B$5:$B$14))^2*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.6806134238997238E-3</v>
       </c>
       <c r="K36">
-        <f t="shared" si="26"/>
+        <f>(Deck!$B10/SUM(Deck!$B$5:$B$14))^2*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.1511501698119817E-4</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B37">
-        <f t="shared" si="24"/>
+        <f>(Deck!$B11/SUM(Deck!$B$5:$B$14))^2*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="C37">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B11/SUM(Deck!$B$5:$B$14))^2*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="D37">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B11/SUM(Deck!$B$5:$B$14))^2*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="E37">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B11/SUM(Deck!$B$5:$B$14))^2*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="F37">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B11/SUM(Deck!$B$5:$B$14))^2*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="G37">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B11/SUM(Deck!$B$5:$B$14))^2*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="H37">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B11/SUM(Deck!$B$5:$B$14))^2*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="I37">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B11/SUM(Deck!$B$5:$B$14))^2*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="J37">
-        <f t="shared" si="25"/>
+        <f>(Deck!$B11/SUM(Deck!$B$5:$B$14))^2*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.6806134238997238E-3</v>
       </c>
       <c r="K37">
-        <f t="shared" si="26"/>
+        <f>(Deck!$B11/SUM(Deck!$B$5:$B$14))^2*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.1511501698119817E-4</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B38">
-        <f t="shared" si="24"/>
+        <f>(Deck!$B12/SUM(Deck!$B$5:$B$14))^2*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="C38">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B12/SUM(Deck!$B$5:$B$14))^2*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="D38">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B12/SUM(Deck!$B$5:$B$14))^2*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="E38">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B12/SUM(Deck!$B$5:$B$14))^2*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="F38">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B12/SUM(Deck!$B$5:$B$14))^2*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="G38">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B12/SUM(Deck!$B$5:$B$14))^2*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="H38">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B12/SUM(Deck!$B$5:$B$14))^2*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="I38">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B12/SUM(Deck!$B$5:$B$14))^2*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="J38">
-        <f t="shared" si="25"/>
+        <f>(Deck!$B12/SUM(Deck!$B$5:$B$14))^2*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.6806134238997238E-3</v>
       </c>
       <c r="K38">
-        <f t="shared" si="26"/>
+        <f>(Deck!$B12/SUM(Deck!$B$5:$B$14))^2*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.1511501698119817E-4</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B39">
-        <f t="shared" si="24"/>
+        <f>(Deck!$B13/SUM(Deck!$B$5:$B$14))^2*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="C39">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B13/SUM(Deck!$B$5:$B$14))^2*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="D39">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B13/SUM(Deck!$B$5:$B$14))^2*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="E39">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B13/SUM(Deck!$B$5:$B$14))^2*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="F39">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B13/SUM(Deck!$B$5:$B$14))^2*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="G39">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B13/SUM(Deck!$B$5:$B$14))^2*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="H39">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B13/SUM(Deck!$B$5:$B$14))^2*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="I39">
-        <f t="shared" si="23"/>
+        <f>(Deck!$B13/SUM(Deck!$B$5:$B$14))^2*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="J39">
-        <f t="shared" si="25"/>
+        <f>(Deck!$B13/SUM(Deck!$B$5:$B$14))^2*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.6806134238997238E-3</v>
       </c>
       <c r="K39">
-        <f t="shared" si="26"/>
+        <f>(Deck!$B13/SUM(Deck!$B$5:$B$14))^2*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.1511501698119817E-4</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B40">
-        <f>(4/13)^2*(1/13)</f>
+        <f>(Deck!$B14/SUM(Deck!$B$5:$B$14))^2*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>7.2826581702321357E-3</v>
       </c>
       <c r="C40">
-        <f t="shared" ref="C40:I40" si="27">(4/13)^2*(1/13)</f>
+        <f>(Deck!$B14/SUM(Deck!$B$5:$B$14))^2*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>7.2826581702321357E-3</v>
       </c>
       <c r="D40">
-        <f t="shared" si="27"/>
+        <f>(Deck!$B14/SUM(Deck!$B$5:$B$14))^2*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>7.2826581702321357E-3</v>
       </c>
       <c r="E40">
-        <f t="shared" si="27"/>
+        <f>(Deck!$B14/SUM(Deck!$B$5:$B$14))^2*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>7.2826581702321357E-3</v>
       </c>
       <c r="F40">
-        <f t="shared" si="27"/>
+        <f>(Deck!$B14/SUM(Deck!$B$5:$B$14))^2*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>7.2826581702321357E-3</v>
       </c>
       <c r="G40">
-        <f t="shared" si="27"/>
+        <f>(Deck!$B14/SUM(Deck!$B$5:$B$14))^2*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>7.2826581702321357E-3</v>
       </c>
       <c r="H40">
-        <f t="shared" si="27"/>
+        <f>(Deck!$B14/SUM(Deck!$B$5:$B$14))^2*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>7.2826581702321357E-3</v>
       </c>
       <c r="I40">
-        <f t="shared" si="27"/>
+        <f>(Deck!$B14/SUM(Deck!$B$5:$B$14))^2*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>7.2826581702321357E-3</v>
       </c>
       <c r="J40">
-        <f>(4/13)^3*(12/13)</f>
+        <f>(Deck!$B14/SUM(Deck!$B$5:$B$14))^2*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>2.688981478239558E-2</v>
       </c>
       <c r="K40">
-        <f>(4/13)^2*(1/13)*(9/13)</f>
+        <f>(Deck!$B14/SUM(Deck!$B$5:$B$14))^2*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>5.0418402716991707E-3</v>
       </c>
     </row>
@@ -13940,43 +13936,43 @@
         <v>10</v>
       </c>
       <c r="B41">
-        <f t="shared" ref="B41:I41" si="28">(1/13)^3</f>
+        <f>(Deck!$B5/SUM(Deck!$B$5:$B$14))^2*(Deck!C$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="C41">
-        <f t="shared" si="28"/>
+        <f>(Deck!$B5/SUM(Deck!$B$5:$B$14))^2*(Deck!D$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="D41">
-        <f t="shared" si="28"/>
+        <f>(Deck!$B5/SUM(Deck!$B$5:$B$14))^2*(Deck!E$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="E41">
-        <f t="shared" si="28"/>
+        <f>(Deck!$B5/SUM(Deck!$B$5:$B$14))^2*(Deck!F$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="F41">
-        <f t="shared" si="28"/>
+        <f>(Deck!$B5/SUM(Deck!$B$5:$B$14))^2*(Deck!G$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="G41">
-        <f t="shared" si="28"/>
+        <f>(Deck!$B5/SUM(Deck!$B$5:$B$14))^2*(Deck!H$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="H41">
-        <f t="shared" si="28"/>
+        <f>(Deck!$B5/SUM(Deck!$B$5:$B$14))^2*(Deck!I$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="I41">
-        <f t="shared" si="28"/>
+        <f>(Deck!$B5/SUM(Deck!$B$5:$B$14))^2*(Deck!J$2/SUM(Deck!$B$2:$K$2))</f>
         <v>4.5516613563950848E-4</v>
       </c>
       <c r="J41">
-        <f>(1/13)^2*(4/13)*(12/13)</f>
+        <f>(Deck!$B5/SUM(Deck!$B$5:$B$14))^2*(Deck!K$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$C$2:$K$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>1.6806134238997238E-3</v>
       </c>
       <c r="K41">
-        <f>(1/13)^3*(9/13)</f>
+        <f>(Deck!$B5/SUM(Deck!$B$5:$B$14))^2*(Deck!B$2/SUM(Deck!$B$2:$K$2))*(SUM(Deck!$B$2:$J$2)/SUM(Deck!$B$2:$K$2))</f>
         <v>3.1511501698119817E-4</v>
       </c>
     </row>
@@ -13993,35 +13989,35 @@
         <v>2</v>
       </c>
       <c r="C45">
-        <f t="shared" ref="C45:J45" si="29">B45+1</f>
+        <f t="shared" ref="C45:J45" si="1">B45+1</f>
         <v>3</v>
       </c>
       <c r="D45">
-        <f t="shared" si="29"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E45">
-        <f t="shared" si="29"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="F45">
-        <f t="shared" si="29"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="G45">
-        <f t="shared" si="29"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H45">
-        <f t="shared" si="29"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I45">
-        <f t="shared" si="29"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J45">
-        <f t="shared" si="29"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="K45" t="s">
@@ -14033,41 +14029,41 @@
         <v>2</v>
       </c>
       <c r="C46">
-        <f t="shared" ref="C46:J54" si="30">$A46+C$45</f>
+        <f t="shared" ref="C46:J54" si="2">$A46+C$45</f>
         <v>5</v>
       </c>
       <c r="D46">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E46">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="F46">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G46">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="H46">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="I46">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="J46">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
-        <f t="shared" ref="A47:A54" si="31">A46+1</f>
+        <f t="shared" ref="A47:A54" si="3">A46+1</f>
         <v>3</v>
       </c>
       <c r="B47">
@@ -14075,297 +14071,297 @@
         <v>5</v>
       </c>
       <c r="D47">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="E47">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="F47">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G47">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="H47">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="I47">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J47">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B48">
-        <f t="shared" ref="B48:B54" si="32">$A48+B$45</f>
+        <f t="shared" ref="B48:B54" si="4">$A48+B$45</f>
         <v>6</v>
       </c>
       <c r="C48">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="E48">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="F48">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G48">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="H48">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="I48">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="J48">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
-        <f t="shared" si="31"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B49">
-        <f t="shared" si="32"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="C49">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="D49">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="F49">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G49">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="H49">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="I49">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J49">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
-        <f t="shared" si="31"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B50">
-        <f t="shared" si="32"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="C50">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="D50">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="E50">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G50">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="H50">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="I50">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="J50">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
-        <f t="shared" si="31"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B51">
-        <f t="shared" si="32"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="C51">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="D51">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="E51">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="F51">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="H51">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="I51">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J51">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
-        <f t="shared" si="31"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B52">
-        <f t="shared" si="32"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="C52">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="D52">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="E52">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="F52">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="G52">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="I52">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="J52">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
-        <f t="shared" si="31"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B53">
-        <f t="shared" si="32"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="C53">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="D53">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="E53">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="F53">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="G53">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="H53">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="J53">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
-        <f t="shared" si="31"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B54">
-        <f t="shared" si="32"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="C54">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="D54">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="E54">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="F54">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G54">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="H54">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="I54">
-        <f t="shared" si="30"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
     </row>
@@ -14392,35 +14388,35 @@
         <v>2</v>
       </c>
       <c r="C60">
-        <f t="shared" ref="C60:J60" si="33">B60+1</f>
+        <f t="shared" ref="C60:J60" si="5">B60+1</f>
         <v>3</v>
       </c>
       <c r="D60">
-        <f t="shared" si="33"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E60">
-        <f t="shared" si="33"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="F60">
-        <f t="shared" si="33"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="G60">
-        <f t="shared" si="33"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="H60">
-        <f t="shared" si="33"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I60">
-        <f t="shared" si="33"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="J60">
-        <f t="shared" si="33"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="K60" t="s">
@@ -14431,372 +14427,340 @@
       <c r="A61">
         <v>2</v>
       </c>
-      <c r="B61">
-        <f>(1/13)^2</f>
+      <c r="C61">
+        <f>Deck!$B6/SUM(Deck!$B$5:$B$14)*Deck!D$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="C61">
-        <f t="shared" ref="C61:I68" si="34">(1/13)^2</f>
+      <c r="D61">
+        <f>Deck!$B6/SUM(Deck!$B$5:$B$14)*Deck!E$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="D61">
-        <f t="shared" si="34"/>
+      <c r="E61">
+        <f>Deck!$B6/SUM(Deck!$B$5:$B$14)*Deck!F$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="E61">
-        <f t="shared" si="34"/>
+      <c r="F61">
+        <f>Deck!$B6/SUM(Deck!$B$5:$B$14)*Deck!G$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="F61">
-        <f t="shared" si="34"/>
+      <c r="G61">
+        <f>Deck!$B6/SUM(Deck!$B$5:$B$14)*Deck!H$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="G61">
-        <f t="shared" si="34"/>
+      <c r="H61">
+        <f>Deck!$B6/SUM(Deck!$B$5:$B$14)*Deck!I$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="H61">
-        <f t="shared" si="34"/>
+      <c r="I61">
+        <f>Deck!$B6/SUM(Deck!$B$5:$B$14)*Deck!J$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="I61">
-        <f t="shared" si="34"/>
-        <v>5.9171597633136102E-3</v>
-      </c>
       <c r="J61">
-        <f t="shared" ref="J61:J68" si="35">(1/13)*(4/13)</f>
+        <f>Deck!$B6/SUM(Deck!$B$5:$B$14)*Deck!K$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
-        <f t="shared" ref="A62:A69" si="36">A61+1</f>
+        <f t="shared" ref="A62:A69" si="6">A61+1</f>
         <v>3</v>
       </c>
       <c r="B62">
-        <f t="shared" ref="B62:B68" si="37">(1/13)^2</f>
+        <f>Deck!$B7/SUM(Deck!$B$5:$B$14)*Deck!C$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="C62">
-        <f t="shared" si="34"/>
+      <c r="D62">
+        <f>Deck!$B7/SUM(Deck!$B$5:$B$14)*Deck!E$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="D62">
-        <f t="shared" si="34"/>
+      <c r="E62">
+        <f>Deck!$B7/SUM(Deck!$B$5:$B$14)*Deck!F$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="E62">
-        <f t="shared" si="34"/>
+      <c r="F62">
+        <f>Deck!$B7/SUM(Deck!$B$5:$B$14)*Deck!G$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="F62">
-        <f t="shared" si="34"/>
+      <c r="G62">
+        <f>Deck!$B7/SUM(Deck!$B$5:$B$14)*Deck!H$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="G62">
-        <f t="shared" si="34"/>
+      <c r="H62">
+        <f>Deck!$B7/SUM(Deck!$B$5:$B$14)*Deck!I$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="H62">
-        <f t="shared" si="34"/>
+      <c r="I62">
+        <f>Deck!$B7/SUM(Deck!$B$5:$B$14)*Deck!J$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="I62">
-        <f t="shared" si="34"/>
-        <v>5.9171597633136102E-3</v>
-      </c>
       <c r="J62">
-        <f t="shared" si="35"/>
+        <f>Deck!$B7/SUM(Deck!$B$5:$B$14)*Deck!K$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
-        <f t="shared" si="36"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="B63">
-        <f t="shared" si="37"/>
+        <f>Deck!$B8/SUM(Deck!$B$5:$B$14)*Deck!C$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="C63">
-        <f t="shared" si="34"/>
+        <f>Deck!$B8/SUM(Deck!$B$5:$B$14)*Deck!D$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="D63">
-        <f t="shared" si="34"/>
+      <c r="E63">
+        <f>Deck!$B8/SUM(Deck!$B$5:$B$14)*Deck!F$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="E63">
-        <f t="shared" si="34"/>
+      <c r="F63">
+        <f>Deck!$B8/SUM(Deck!$B$5:$B$14)*Deck!G$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="F63">
-        <f t="shared" si="34"/>
+      <c r="G63">
+        <f>Deck!$B8/SUM(Deck!$B$5:$B$14)*Deck!H$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="G63">
-        <f t="shared" si="34"/>
+      <c r="H63">
+        <f>Deck!$B8/SUM(Deck!$B$5:$B$14)*Deck!I$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="H63">
-        <f t="shared" si="34"/>
+      <c r="I63">
+        <f>Deck!$B8/SUM(Deck!$B$5:$B$14)*Deck!J$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="I63">
-        <f t="shared" si="34"/>
-        <v>5.9171597633136102E-3</v>
-      </c>
       <c r="J63">
-        <f t="shared" si="35"/>
+        <f>Deck!$B8/SUM(Deck!$B$5:$B$14)*Deck!K$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
-        <f t="shared" si="36"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="B64">
-        <f t="shared" si="37"/>
+        <f>Deck!$B9/SUM(Deck!$B$5:$B$14)*Deck!C$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="C64">
-        <f t="shared" si="34"/>
+        <f>Deck!$B9/SUM(Deck!$B$5:$B$14)*Deck!D$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="D64">
-        <f t="shared" si="34"/>
+        <f>Deck!$B9/SUM(Deck!$B$5:$B$14)*Deck!E$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="E64">
-        <f t="shared" si="34"/>
+      <c r="F64">
+        <f>Deck!$B9/SUM(Deck!$B$5:$B$14)*Deck!G$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="F64">
-        <f t="shared" si="34"/>
+      <c r="G64">
+        <f>Deck!$B9/SUM(Deck!$B$5:$B$14)*Deck!H$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="G64">
-        <f t="shared" si="34"/>
+      <c r="H64">
+        <f>Deck!$B9/SUM(Deck!$B$5:$B$14)*Deck!I$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="H64">
-        <f t="shared" si="34"/>
+      <c r="I64">
+        <f>Deck!$B9/SUM(Deck!$B$5:$B$14)*Deck!J$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="I64">
-        <f t="shared" si="34"/>
-        <v>5.9171597633136102E-3</v>
-      </c>
       <c r="J64">
-        <f t="shared" si="35"/>
+        <f>Deck!$B9/SUM(Deck!$B$5:$B$14)*Deck!K$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
-        <f t="shared" si="36"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="B65">
-        <f t="shared" si="37"/>
+        <f>Deck!$B10/SUM(Deck!$B$5:$B$14)*Deck!C$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="C65">
-        <f t="shared" si="34"/>
+        <f>Deck!$B10/SUM(Deck!$B$5:$B$14)*Deck!D$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="D65">
-        <f t="shared" si="34"/>
+        <f>Deck!$B10/SUM(Deck!$B$5:$B$14)*Deck!E$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="E65">
-        <f t="shared" si="34"/>
+        <f>Deck!$B10/SUM(Deck!$B$5:$B$14)*Deck!F$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="F65">
-        <f t="shared" si="34"/>
+      <c r="G65">
+        <f>Deck!$B10/SUM(Deck!$B$5:$B$14)*Deck!H$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="G65">
-        <f t="shared" si="34"/>
+      <c r="H65">
+        <f>Deck!$B10/SUM(Deck!$B$5:$B$14)*Deck!I$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="H65">
-        <f t="shared" si="34"/>
+      <c r="I65">
+        <f>Deck!$B10/SUM(Deck!$B$5:$B$14)*Deck!J$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="I65">
-        <f t="shared" si="34"/>
-        <v>5.9171597633136102E-3</v>
-      </c>
       <c r="J65">
-        <f t="shared" si="35"/>
+        <f>Deck!$B10/SUM(Deck!$B$5:$B$14)*Deck!K$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
-        <f t="shared" si="36"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="B66">
-        <f t="shared" si="37"/>
+        <f>Deck!$B11/SUM(Deck!$B$5:$B$14)*Deck!C$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="C66">
-        <f t="shared" si="34"/>
+        <f>Deck!$B11/SUM(Deck!$B$5:$B$14)*Deck!D$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="D66">
-        <f t="shared" si="34"/>
+        <f>Deck!$B11/SUM(Deck!$B$5:$B$14)*Deck!E$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="E66">
-        <f t="shared" si="34"/>
+        <f>Deck!$B11/SUM(Deck!$B$5:$B$14)*Deck!F$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="F66">
-        <f t="shared" si="34"/>
+        <f>Deck!$B11/SUM(Deck!$B$5:$B$14)*Deck!G$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="G66">
-        <f t="shared" si="34"/>
+      <c r="H66">
+        <f>Deck!$B11/SUM(Deck!$B$5:$B$14)*Deck!I$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="H66">
-        <f t="shared" si="34"/>
+      <c r="I66">
+        <f>Deck!$B11/SUM(Deck!$B$5:$B$14)*Deck!J$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="I66">
-        <f t="shared" si="34"/>
-        <v>5.9171597633136102E-3</v>
-      </c>
       <c r="J66">
-        <f t="shared" si="35"/>
+        <f>Deck!$B11/SUM(Deck!$B$5:$B$14)*Deck!K$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
-        <f t="shared" si="36"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="B67">
-        <f t="shared" si="37"/>
+        <f>Deck!$B12/SUM(Deck!$B$5:$B$14)*Deck!C$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="C67">
-        <f t="shared" si="34"/>
+        <f>Deck!$B12/SUM(Deck!$B$5:$B$14)*Deck!D$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="D67">
-        <f t="shared" si="34"/>
+        <f>Deck!$B12/SUM(Deck!$B$5:$B$14)*Deck!E$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="E67">
-        <f t="shared" si="34"/>
+        <f>Deck!$B12/SUM(Deck!$B$5:$B$14)*Deck!F$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="F67">
-        <f t="shared" si="34"/>
+        <f>Deck!$B12/SUM(Deck!$B$5:$B$14)*Deck!G$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="G67">
-        <f t="shared" si="34"/>
+        <f>Deck!$B12/SUM(Deck!$B$5:$B$14)*Deck!H$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="H67">
-        <f t="shared" si="34"/>
+      <c r="I67">
+        <f>Deck!$B12/SUM(Deck!$B$5:$B$14)*Deck!J$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="I67">
-        <f t="shared" si="34"/>
-        <v>5.9171597633136102E-3</v>
-      </c>
       <c r="J67">
-        <f t="shared" si="35"/>
+        <f>Deck!$B12/SUM(Deck!$B$5:$B$14)*Deck!K$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
-        <f t="shared" si="36"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="B68">
-        <f t="shared" si="37"/>
+        <f>Deck!$B13/SUM(Deck!$B$5:$B$14)*Deck!C$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="C68">
-        <f t="shared" si="34"/>
+        <f>Deck!$B13/SUM(Deck!$B$5:$B$14)*Deck!D$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="D68">
-        <f t="shared" si="34"/>
+        <f>Deck!$B13/SUM(Deck!$B$5:$B$14)*Deck!E$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="E68">
-        <f t="shared" si="34"/>
+        <f>Deck!$B13/SUM(Deck!$B$5:$B$14)*Deck!F$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="F68">
-        <f t="shared" si="34"/>
+        <f>Deck!$B13/SUM(Deck!$B$5:$B$14)*Deck!G$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="G68">
-        <f t="shared" si="34"/>
+        <f>Deck!$B13/SUM(Deck!$B$5:$B$14)*Deck!H$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
       <c r="H68">
-        <f t="shared" si="34"/>
+        <f>Deck!$B13/SUM(Deck!$B$5:$B$14)*Deck!I$2/SUM(Deck!$B$5:$B$14)</f>
         <v>5.9171597633136102E-3</v>
       </c>
-      <c r="I68">
-        <f t="shared" si="34"/>
-        <v>5.9171597633136102E-3</v>
-      </c>
       <c r="J68">
-        <f t="shared" si="35"/>
+        <f>Deck!$B13/SUM(Deck!$B$5:$B$14)*Deck!K$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
-        <f t="shared" si="36"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="B69">
-        <f>(1/13)*(4/13)</f>
+        <f>Deck!$B14/SUM(Deck!$B$5:$B$14)*Deck!C$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
       <c r="C69">
-        <f t="shared" ref="C69:I69" si="38">(1/13)*(4/13)</f>
+        <f>Deck!$B14/SUM(Deck!$B$5:$B$14)*Deck!D$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
       <c r="D69">
-        <f t="shared" si="38"/>
+        <f>Deck!$B14/SUM(Deck!$B$5:$B$14)*Deck!E$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
       <c r="E69">
-        <f t="shared" si="38"/>
+        <f>Deck!$B14/SUM(Deck!$B$5:$B$14)*Deck!F$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
       <c r="F69">
-        <f t="shared" si="38"/>
+        <f>Deck!$B14/SUM(Deck!$B$5:$B$14)*Deck!G$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
       <c r="G69">
-        <f t="shared" si="38"/>
+        <f>Deck!$B14/SUM(Deck!$B$5:$B$14)*Deck!H$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
       <c r="H69">
-        <f t="shared" si="38"/>
+        <f>Deck!$B14/SUM(Deck!$B$5:$B$14)*Deck!I$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
       <c r="I69">
-        <f t="shared" si="38"/>
+        <f>Deck!$B14/SUM(Deck!$B$5:$B$14)*Deck!J$2/SUM(Deck!$B$5:$B$14)</f>
         <v>2.3668639053254441E-2</v>
       </c>
     </row>
@@ -14834,7 +14798,7 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79">
-        <f t="shared" ref="A79:A92" si="39">A78+1</f>
+        <f t="shared" ref="A79:A92" si="7">A78+1</f>
         <v>7</v>
       </c>
       <c r="B79">
@@ -14844,7 +14808,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80">
-        <f t="shared" si="39"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="B80">
@@ -14854,7 +14818,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
-        <f t="shared" si="39"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="B81">
@@ -14864,7 +14828,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="B82">
@@ -14874,7 +14838,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
-        <f t="shared" si="39"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="B83">
@@ -14884,7 +14848,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
-        <f t="shared" si="39"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="B84">
@@ -14894,7 +14858,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
-        <f t="shared" si="39"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="B85">
@@ -14904,7 +14868,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
-        <f t="shared" si="39"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
       <c r="B86">
@@ -14914,7 +14878,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
-        <f t="shared" si="39"/>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="B87">
@@ -14924,7 +14888,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
-        <f t="shared" si="39"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="B88">
@@ -14934,7 +14898,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
-        <f t="shared" si="39"/>
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
       <c r="B89">
@@ -14944,7 +14908,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
-        <f t="shared" si="39"/>
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
       <c r="B90">
@@ -14954,7 +14918,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
-        <f t="shared" si="39"/>
+        <f t="shared" si="7"/>
         <v>19</v>
       </c>
       <c r="B91">
@@ -14964,7 +14928,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
-        <f t="shared" si="39"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="B92">
@@ -14981,8 +14945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16591,8 +16555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19283,7 +19247,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>